<commit_message>
se añade reporte de bugs
</commit_message>
<xml_diff>
--- a/Casos-de-Prueba.xlsx
+++ b/Casos-de-Prueba.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AA1425C-20DD-4284-BCC1-F6A446696BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCA5F660-125E-43D2-BAF0-0E72CFCE856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="2" r:id="rId1"/>
     <sheet name="Login" sheetId="1" r:id="rId2"/>
     <sheet name="Lista de Productos" sheetId="3" r:id="rId3"/>
     <sheet name="Carrito" sheetId="4" r:id="rId4"/>
+    <sheet name="Checkout" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="185">
   <si>
     <t>Test Scenarios ID</t>
   </si>
@@ -457,14 +458,288 @@
     <t>TC_022</t>
   </si>
   <si>
-    <t>standar_user</t>
+    <t>Validar que un producto es añadido correctamente al carrito desde el listado de productos</t>
+  </si>
+  <si>
+    <t>1.Click en "Add to cart" del producto "Sauce Labs Backpacks"
+2.Abrir el Carrito
+3. Verificar que el producto se encuentra en el carrito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El producto es añadido al carrito
+El boton "Add to cart" cambio a  "Remove"
+</t>
+  </si>
+  <si>
+    <t>El producto es añadido al carrito
+El boton "Add to cart" cambio a "Remove"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar que el usuario pueda añadir el producto al carrito desde la descripcion de un producto </t>
+  </si>
+  <si>
+    <t>1.Click en el nombre del Producto 
+2.Click en "Add to cart" 
+3.Abrir el Carrito
+4. Verificar que el producto se encuentra en el carrito</t>
+  </si>
+  <si>
+    <t>El producto es añadido al carrito
+El boton "Add to cart" cambio a  "Remove"</t>
+  </si>
+  <si>
+    <t>Validar que multiples productos pueden ser añadidos al carrito desde el listado de productos</t>
+  </si>
+  <si>
+    <t>1.Click en "Add to cart" en la parte inferior derecha de un producto
+2.Click en "Add to cart" en el siguiente producto de la lista 
+3.Abrir el Carrito
+4. Verificar que el producto se encuentra en el carrito</t>
+  </si>
+  <si>
+    <t>Ambos productos deberian aparecer listados en el carrito</t>
+  </si>
+  <si>
+    <t>Se muestran correctamente los dos productos añadidos en el carrito</t>
+  </si>
+  <si>
+    <t>Validar que el usuario pueda remover productos desde el listado de productos</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/
+Estar logeado con:
+standard_user
+tener elementos añadidos al carrito</t>
+  </si>
+  <si>
+    <t>1. Identificar un producto que ya tenga el boton "Remove" 
+2. Click en el boton "Remove" 
+3.Verificar que el botón vuelve a mostrar la opción "Add to Cart" 
+4.Confirmar que el producto ya no aparece en el carrito</t>
+  </si>
+  <si>
+    <t>El boton cambia de "Remove" a "Add to Cart" 
+El producto ya no aparece en el carrito</t>
+  </si>
+  <si>
+    <t>Validar que el contador del Carrito cambie correctamente al agregar o remover productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.saucedemo.com/
+Estar logeado con:
+standard_user
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verificar que el contador del carrito no se muestra (0 items)
+2.Hacer click en "Add to Cart" en un producto
+3.Verificar que el contador del carrito muestre 1
+4.Hacer click en "Add to Cart" en un segundo producto
+5.Verificar que el contador del carrito muestre 2
+6.Hacer Click en "Remove" en uno de los productos
+7.Verificar que el contador del carrito muestre 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Contador del carrito incrementa al agregar productos
+El contador decrementa correctamente al remover productos
+</t>
+  </si>
+  <si>
+    <t>Validar que los productos son añadidos al carrito</t>
+  </si>
+  <si>
+    <t>1.Click en el nombre del Producto "Sauce Labs Backpack" 
+2.Click en "Add to cart" 
+3.Abrir el Carrito
+4. Verificar que el producto se encuentra en el carrito</t>
+  </si>
+  <si>
+    <t>El boton "Add to cart" no añade el producto al carrito
+El boton "Add to cart" no cambio a "Remove"</t>
+  </si>
+  <si>
+    <t>El boton no cambia de "Remove" a "Add to Cart" 
+El producto sigue en el carrito</t>
+  </si>
+  <si>
+    <t>El contador del carrito incrementa al agregar productos 
+El contador no decrementa correctamente debido a que no se puede remover los productos</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/
+Estar logeado con:
+error_user</t>
+  </si>
+  <si>
+    <t>Validar que el usuario pueda iniciar el proceso del Checkout</t>
+  </si>
+  <si>
+    <t>1.Hacer click en el carrito
+2.Click en el boton "Checkout"</t>
+  </si>
+  <si>
+    <t>El usuario es rederigido a la pantalla de Checkout: Your Information</t>
+  </si>
+  <si>
+    <t>Validar que el usuario haya ingresado credenciales validas en los campos requeridos</t>
+  </si>
+  <si>
+    <t>First Name: Luan
+Last Name: Acevedo
+Zip: 5012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Hacer click en el carrito
+2. Click en el boton "Checkout"
+3.Completar First Name
+4.Completar Last Name
+5.Completar  Codigo Postal/ZIP
+6.Click en el boton "Continue"
+</t>
+  </si>
+  <si>
+    <t>El usuario es rederigido a la pantalla de Checkout: Overview</t>
+  </si>
+  <si>
+    <t>El usuario es rederigido correctamente a "Checkout:Overview"</t>
+  </si>
+  <si>
+    <t>Validar que el sitema muestre un error cuando un campo "First Name" se deja vacio en el Checkout</t>
+  </si>
+  <si>
+    <t>First Name: NA
+Last Name: Acevedo
+Zip: 5012</t>
+  </si>
+  <si>
+    <t>1.Hacer click en el carrito
+2.Click en el boton "Checkout"
+3.Dejar el campo "First Name" vacio
+4.Completar "Last Name" 
+5. Completar"Postal Code / ZIP"
+6. Click en el boton "Continue"</t>
+  </si>
+  <si>
+    <t>El sistema no permite avanzar al siguiente paso del checkout
+Mensaje de error visible: 
+"Error: First Name is required"</t>
+  </si>
+  <si>
+    <t>Validar que el sitema muestre un error cuando un campo "Last Name" se deja vacio en el Checkout</t>
+  </si>
+  <si>
+    <t>First Name: Luan
+Last Name: NA
+Zip: 5012</t>
+  </si>
+  <si>
+    <t>1.Hacer click en el carrito
+2.Click en el boton "Checkout"
+3.Completar "First Name"
+4.Dejar el campo "Last Name" vacio
+5. Completar"Postal Code / ZIP"
+6. Click en el boton "Continue"</t>
+  </si>
+  <si>
+    <t>El sistema no permite avanzar al siguiente paso del checkout
+Mensaje de error visible: 
+"Error: Last Name is required"</t>
+  </si>
+  <si>
+    <t>Validar que el sitema muestre un error cuando un campo "Zip/Postal Code" se deja vacio en el Checkout</t>
+  </si>
+  <si>
+    <t>First Name: Luan
+Last Name: Acevedo
+Zip: NA</t>
+  </si>
+  <si>
+    <t>1.Hacer click en el carrito
+2.Click en el boton "Checkout"
+3.Completar "First Name"
+4.Dejar el campo "Last Name" vacio
+5. Dejar el campo "Postal Code / ZIP" vacio
+6. Click en el boton "Continue"</t>
+  </si>
+  <si>
+    <t>El sistema no permite avanzar al siguiente paso del checkout
+Mensaje de error visible: 
+"Error: Postal Code is required"</t>
+  </si>
+  <si>
+    <t>Validar que el boton "Cancelar" redigira a la pagina del carrito</t>
+  </si>
+  <si>
+    <t>1.Hacer click en el carrito
+2.Hacer click en el boton "Checkout"
+3.Hacer click en el boton "Cancel"</t>
+  </si>
+  <si>
+    <t>El usuario es rederigido a la pagina del Carrito</t>
+  </si>
+  <si>
+    <t>Validar Mensaje de finalazacion de compra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Hacer click en el carrito
+2. Click en el boton "Checkout"
+3.Completar First Name
+4.Completar Last Name
+5.Completar  Codigo Postal/ZIP
+6.Click en el boton "Continue"
+7.Click en el boton "Finish"
+</t>
+  </si>
+  <si>
+    <t>El usuario es rederigido a la pagina "Checkout: Complete!" 
+Aparece mensaje visibible de confirmacion de compra "Thanks you for your order!"</t>
+  </si>
+  <si>
+    <t>El campo "Last Name" no se puede completar y modifica el campo "First Name"
+El usuario no es rederigido a la pantalla de Checkout:Overview</t>
+  </si>
+  <si>
+    <t>El campo "Last Name" no se puede completar y modifica el campo "First Name"
+Mensaje de error visible:
+"Error: Last Name is required"</t>
+  </si>
+  <si>
+    <t>El campo "Last Name" no se puede completar y modifica el campo "First Name"
+El usuario no es rederigido a la pantalla de Checkout:Overview , no se puede seguir con la prueba</t>
+  </si>
+  <si>
+    <t>El campo "Last Name" no se puede completar y el usuario es rederigido  a "Checkout:Overview"</t>
+  </si>
+  <si>
+    <t>El campo "Last Name" no se puede completar 
+Mensaje de error visible: 
+"Error: First Name is required"
+El usuario no es rederigido a la pantalla de Checkout:Overview</t>
+  </si>
+  <si>
+    <t>First Name: Acevedo Luan
+Last Name: NA
+Zip: 5012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema redirecciona a "Checkout: Overview" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El campo "Last Name" no se puede completar 
+</t>
+  </si>
+  <si>
+    <t>El campo "Last Name" no se puede completar
+El usuario  es rederigido a la pantalla de Checkout:Overview
+El boton "Finish" no redirecciona a la siguente pestaña</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +760,14 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -570,7 +853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -592,6 +875,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -929,7 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE5D9DD-79F1-4BC7-80CC-E6C912053B00}">
   <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -979,7 +1266,9 @@
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
@@ -991,7 +1280,9 @@
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
@@ -1003,7 +1294,9 @@
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1014,7 +1307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
@@ -1632,7 +1925,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2335,19 +2628,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B733F9-3727-42BE-A243-D14A1004108B}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2381,8 +2675,1133 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="15" customFormat="1" ht="72.75">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>125</v>
       </c>
+      <c r="D4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="72.75">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="101.25">
+      <c r="A6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="101.25">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="216.75">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="72.75">
+      <c r="A11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="87">
+      <c r="A12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="101.25">
+      <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="101.25">
+      <c r="A14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="216.75">
+      <c r="A15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="72.75">
+      <c r="A18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="87">
+      <c r="A19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="101.25">
+      <c r="A20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="101.25">
+      <c r="A21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="216.75">
+      <c r="A22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13871F2A-1B82-423B-80EF-118EB378D55F}">
+  <dimension ref="A1:J34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.5">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="101.25">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="101.25">
+      <c r="A6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="101.25">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="115.5">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="72.75">
+      <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="115.5">
+      <c r="A10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="43.5">
+      <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="101.25">
+      <c r="A14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="101.25">
+      <c r="A15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="101.25">
+      <c r="A16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="115.5">
+      <c r="A17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="72.75">
+      <c r="A18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="115.5">
+      <c r="A19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="43.5">
+      <c r="A22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="101.25">
+      <c r="A23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="101.25">
+      <c r="A24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="101.25">
+      <c r="A25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="115.5">
+      <c r="A26" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="72.75">
+      <c r="A27" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="115.5">
+      <c r="A28" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10">
+      <c r="J34" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>